<commit_message>
Changes to be committed: 	modified:   .gitignore 	modified:   README.md 	modified:   answer_generator.py 	modified:   category_filler.py 	modified:   db/duckdb_qa_store.py 	modified:   db/duckdb_qa_store_test.py 	modified:   docs/Q-REPLY_REQ.md 	modified:   embeddings/base_embedding.py 	modified:   gigachat/__init__.py 	modified:   gigachat/client.py 	modified:   gigachat/config.py 	new file:   in/Q.origin.xlsx 	deleted:    in/Q.xlsx 	modified:   in/QA.origin.xlsx 	deleted:    in/QA.xlsx 	deleted:    out/QA_2025-08-28_151223.xlsx 	deleted:    out/QA_2025-08-28_151435.xlsx 	deleted:    out/Q_2025-08-28_151921.xlsx 	modified:   prompts/README.md 	modified:   prompts/base_prompt.py 	modified:   prompts/get_answer_prompt.py 	renamed:    prompts/define_category_prompt.py -> prompts/get_category_prompt.py 	new file:   pyproject.toml 	modified:   update_db.py
</commit_message>
<xml_diff>
--- a/in/QA.origin.xlsx
+++ b/in/QA.origin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -281,12 +281,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -310,9 +319,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -597,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,19 +1031,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to be committed: 	deleted:    _db/README.md 	deleted:    _db/__init__.py 	deleted:    _db/duckdb_qa_store.py 	deleted:    _db/duckdb_qa_store_test.py 	modified:   category_filler.py 	modified:   in/QA.origin.xlsx 	modified:   update_db.py
</commit_message>
<xml_diff>
--- a/in/QA.origin.xlsx
+++ b/in/QA.origin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>Категория</t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t>эканомика</t>
+  </si>
+  <si>
+    <t>Какие решения для работы с большими данными используются в энергетической отрасли?</t>
+  </si>
+  <si>
+    <t>Опишите этапы запуска системы предсказательного мониторинга состояния активов</t>
+  </si>
+  <si>
+    <t>Что должен знать персонал энергокомпаний в эпоху цифровизации?</t>
   </si>
 </sst>
 </file>
@@ -607,16 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="81.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="97" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -632,334 +641,349 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -972,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>

</xml_diff>